<commit_message>
Changing the single tension-pCa fitting demo
</commit_message>
<xml_diff>
--- a/demo_files/fitting/pCa_curve_single/target_data/target_force_pCa_data.xlsx
+++ b/demo_files/fitting/pCa_curve_single/target_data/target_force_pCa_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\GitHub\FiberSim\code\FiberPy\FiberPy\package\demo_files\fitting\pCa_curve_single\target_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sako231\OneDrive - University of Kentucky\Documents\GitHub\FiberSim\demo_files\fitting\pCa_curve_single\target_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBE2C42-4E21-4FB9-BF47-FCCC1D4BD164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{4DBE2C42-4E21-4FB9-BF47-FCCC1D4BD164}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BB7C529-CFF6-4986-AB9B-AE434C9B8FE9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>SL</t>
-  </si>
-  <si>
-    <t>1.9</t>
   </si>
   <si>
     <t>pCa</t>
@@ -34,10 +31,10 @@
     <t>force</t>
   </si>
   <si>
-    <t>force_error</t>
+    <t>curve</t>
   </si>
   <si>
-    <t>curve</t>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -397,49 +394,44 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>782</v>
-      </c>
-      <c r="E2">
-        <v>149.33184523068078</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -447,16 +439,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>1522</v>
-      </c>
-      <c r="E3">
-        <v>738.66997592519851</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -464,16 +453,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="D4">
-        <v>13930</v>
-      </c>
-      <c r="E4">
-        <v>1518.1823927900687</v>
+        <v>59000</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -481,16 +467,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>5.4</v>
       </c>
       <c r="D5">
-        <v>38000</v>
-      </c>
-      <c r="E5">
-        <v>1556.5917183956037</v>
+        <v>140000</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -498,16 +481,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="D6">
-        <v>39500</v>
-      </c>
-      <c r="E6">
-        <v>2227.0633379208398</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -601,7 +581,7 @@
       <c r="B36" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E39">
+  <sortState ref="A2:E39">
     <sortCondition descending="1" ref="C2:C39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>